<commit_message>
Third commit. Adding hooks.
</commit_message>
<xml_diff>
--- a/src/main/java/com/renderz/datafiles/prices.xlsx
+++ b/src/main/java/com/renderz/datafiles/prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="87">
   <si>
     <t xml:space="preserve">Player</t>
   </si>
@@ -242,6 +242,45 @@
   </si>
   <si>
     <t>42,100</t>
+  </si>
+  <si>
+    <t>37,600</t>
+  </si>
+  <si>
+    <t>41,500</t>
+  </si>
+  <si>
+    <t>34,200</t>
+  </si>
+  <si>
+    <t>37,800</t>
+  </si>
+  <si>
+    <t>34,000</t>
+  </si>
+  <si>
+    <t>37,500</t>
+  </si>
+  <si>
+    <t>35,600</t>
+  </si>
+  <si>
+    <t>38,600</t>
+  </si>
+  <si>
+    <t>42,700</t>
+  </si>
+  <si>
+    <t>38,800</t>
+  </si>
+  <si>
+    <t>42,900</t>
+  </si>
+  <si>
+    <t>38,200</t>
+  </si>
+  <si>
+    <t>42,300</t>
   </si>
 </sst>
 </file>
@@ -362,10 +401,10 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,10 +412,10 @@
         <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,10 +423,10 @@
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,10 +434,10 @@
         <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,10 +456,10 @@
         <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,37 +467,37 @@
         <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
         <v>36</v>
@@ -469,7 +508,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -480,7 +519,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -491,18 +530,18 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
         <v>36</v>
@@ -513,18 +552,18 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -535,7 +574,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -546,7 +585,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
         <v>36</v>
@@ -557,18 +596,18 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -579,7 +618,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -590,13 +629,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fourth commit: add re-run feature for failed tc.
</commit_message>
<xml_diff>
--- a/src/main/java/com/renderz/datafiles/prices.xlsx
+++ b/src/main/java/com/renderz/datafiles/prices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="105">
   <si>
     <t xml:space="preserve">Player</t>
   </si>
@@ -281,6 +281,60 @@
   </si>
   <si>
     <t>42,300</t>
+  </si>
+  <si>
+    <t>31,300</t>
+  </si>
+  <si>
+    <t>34,600</t>
+  </si>
+  <si>
+    <t>31,100</t>
+  </si>
+  <si>
+    <t>34,400</t>
+  </si>
+  <si>
+    <t>38,500</t>
+  </si>
+  <si>
+    <t>42,600</t>
+  </si>
+  <si>
+    <t>30,000</t>
+  </si>
+  <si>
+    <t>33,100</t>
+  </si>
+  <si>
+    <t>38,300</t>
+  </si>
+  <si>
+    <t>42,400</t>
+  </si>
+  <si>
+    <t>30,400</t>
+  </si>
+  <si>
+    <t>33,600</t>
+  </si>
+  <si>
+    <t>32,700</t>
+  </si>
+  <si>
+    <t>36,200</t>
+  </si>
+  <si>
+    <t>29,000</t>
+  </si>
+  <si>
+    <t>32,100</t>
+  </si>
+  <si>
+    <t>29,900</t>
+  </si>
+  <si>
+    <t>33,000</t>
   </si>
 </sst>
 </file>
@@ -401,70 +455,70 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
         <v>36</v>
@@ -475,40 +529,40 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
@@ -519,62 +573,62 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>36</v>
@@ -596,7 +650,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>36</v>
@@ -607,7 +661,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -618,7 +672,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
@@ -629,13 +683,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>